<commit_message>
changed comparison color code
</commit_message>
<xml_diff>
--- a/object_detection/TFLITE_PERF_TEST-COMPARISON.xlsx
+++ b/object_detection/TFLITE_PERF_TEST-COMPARISON.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ACCELR_internship\github\tflite-perf-tests\object_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9EF995-AAED-4257-971D-65D514D64868}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BA9147-9799-46D6-A714-53C7C9F3A6E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -177,12 +177,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -213,38 +207,44 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF9900"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -304,25 +304,57 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -331,38 +363,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -584,8 +584,8 @@
   </sheetPr>
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="65" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -601,208 +601,208 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
     </row>
     <row r="3" spans="1:24" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="34" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="35" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="35"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="28"/>
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="31" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="36" t="s">
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="31" t="s">
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="36" t="s">
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="27" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="23" t="s">
+      <c r="G5" s="14"/>
+      <c r="H5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="24"/>
-      <c r="J5" s="25" t="s">
+      <c r="I5" s="14"/>
+      <c r="J5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="29" t="s">
+      <c r="M5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="25" t="s">
+      <c r="N5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="25" t="s">
+      <c r="O5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="23" t="s">
+      <c r="P5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="23" t="s">
+      <c r="Q5" s="14"/>
+      <c r="R5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="24"/>
-      <c r="T5" s="25" t="s">
+      <c r="S5" s="14"/>
+      <c r="T5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="U5" s="25" t="s">
+      <c r="U5" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="14" t="s">
+      <c r="A6" s="14"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="14" t="s">
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="13" t="s">
+      <c r="Q6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="R6" s="14" t="s">
+      <c r="R6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="13" t="s">
+      <c r="S6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -1194,67 +1194,67 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="30">
         <v>11.8931</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="30">
         <v>12.122400000000001</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="12">
+      <c r="D13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="30">
         <v>12.7692</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="30">
         <v>12.327500000000001</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="30">
         <v>12.488799999999999</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="30">
         <v>11.545500000000001</v>
       </c>
-      <c r="J13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L13" s="12">
+      <c r="J13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="30">
         <v>14.611000000000001</v>
       </c>
-      <c r="M13" s="12">
+      <c r="M13" s="30">
         <v>15.1486</v>
       </c>
-      <c r="N13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="P13" s="12">
+      <c r="N13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" s="30">
         <v>15.7567</v>
       </c>
-      <c r="Q13" s="12">
+      <c r="Q13" s="30">
         <v>14.2964</v>
       </c>
-      <c r="R13" s="12">
+      <c r="R13" s="30">
         <v>14.9931</v>
       </c>
-      <c r="S13" s="12">
+      <c r="S13" s="30">
         <v>13.837400000000001</v>
       </c>
-      <c r="T13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="U13" s="11" t="s">
+      <c r="T13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="U13" s="29" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1389,132 +1389,132 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="31">
         <v>15.230700000000001</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="30">
         <v>15.8794</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="22">
+      <c r="D16" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="36">
         <v>15.3744</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="31">
         <v>15.2136</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="31">
         <v>15.010300000000001</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="31">
         <v>14.070600000000001</v>
       </c>
-      <c r="J16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L16" s="12">
+      <c r="J16" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="30">
         <v>18.652899999999999</v>
       </c>
-      <c r="M16" s="12">
+      <c r="M16" s="30">
         <v>19.4072</v>
       </c>
-      <c r="N16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="P16" s="18">
+      <c r="N16" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="P16" s="31">
         <v>19.525500000000001</v>
       </c>
-      <c r="Q16" s="22">
+      <c r="Q16" s="36">
         <v>19.202500000000001</v>
       </c>
-      <c r="R16" s="12">
+      <c r="R16" s="30">
         <v>17.069099999999999</v>
       </c>
-      <c r="S16" s="18">
+      <c r="S16" s="31">
         <v>18.8599</v>
       </c>
-      <c r="T16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="U16" s="11" t="s">
+      <c r="T16" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="U16" s="29" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="34">
         <v>14.939500000000001</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="37">
         <v>15.9551</v>
       </c>
-      <c r="D17" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="17">
+      <c r="D17" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="35">
         <v>13.662800000000001</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="34">
         <v>13.752000000000001</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="34">
         <v>13.3429</v>
       </c>
-      <c r="I17" s="16">
+      <c r="I17" s="34">
         <v>13.536799999999999</v>
       </c>
-      <c r="J17" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="L17" s="19">
+      <c r="J17" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="32">
         <v>18.9712</v>
       </c>
-      <c r="M17" s="21">
+      <c r="M17" s="37">
         <v>19.6126</v>
       </c>
-      <c r="N17" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="O17" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="P17" s="16">
+      <c r="N17" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="O17" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="P17" s="34">
         <v>18.937200000000001</v>
       </c>
-      <c r="Q17" s="16">
+      <c r="Q17" s="34">
         <v>19.0989</v>
       </c>
-      <c r="R17" s="19">
+      <c r="R17" s="32">
         <v>17.856100000000001</v>
       </c>
-      <c r="S17" s="16">
+      <c r="S17" s="34">
         <v>17.753299999999999</v>
       </c>
-      <c r="T17" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="U17" s="15" t="s">
+      <c r="T17" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="U17" s="33" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1698,7 +1698,7 @@
       <c r="Q20" s="7">
         <v>35.758699999999997</v>
       </c>
-      <c r="R20" s="20">
+      <c r="R20" s="38">
         <v>53.032899999999998</v>
       </c>
       <c r="S20" s="6">
@@ -1727,15 +1727,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:K4"/>
     <mergeCell ref="R5:S5"/>
     <mergeCell ref="T5:T6"/>
     <mergeCell ref="U5:U6"/>
@@ -1752,6 +1743,15 @@
     <mergeCell ref="P4:U4"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
detector, object_detection.py that supports coco_eval are added
</commit_message>
<xml_diff>
--- a/object_detection/TFLITE_PERF_TEST-COMPARISON.xlsx
+++ b/object_detection/TFLITE_PERF_TEST-COMPARISON.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ACCELR_internship\github\tflite-perf-tests\object_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BA9147-9799-46D6-A714-53C7C9F3A6E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53771087-FCCC-44C1-9E88-901F83A861D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="156" windowWidth="11724" windowHeight="11592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="38">
   <si>
     <t>TFLITE-COMPARISON</t>
   </si>
@@ -116,13 +116,43 @@
   </si>
   <si>
     <t>10. example (they given for CPP)</t>
+  </si>
+  <si>
+    <t>ssd_mobilenet_v1_default_model</t>
+  </si>
+  <si>
+    <t>coco_ssd_mobilenet_v1_1_model</t>
+  </si>
+  <si>
+    <t>IOU=0.50:0.95</t>
+  </si>
+  <si>
+    <t>IOU=0.50</t>
+  </si>
+  <si>
+    <t>IOU=0.75</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AVERAGE PRECISION- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>BASELINES</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -158,6 +188,25 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF212121"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -284,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -306,64 +355,72 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,10 +639,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X24"/>
+  <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="65" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -601,176 +658,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
     </row>
     <row r="3" spans="1:24" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="38"/>
+      <c r="B3" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="28" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="21" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23" t="s">
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="21" t="s">
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="23" t="s">
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="20" t="s">
+      <c r="G5" s="24"/>
+      <c r="H5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="13" t="s">
+      <c r="I5" s="24"/>
+      <c r="J5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="M5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="N5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="13" t="s">
+      <c r="O5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="P5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="20" t="s">
+      <c r="Q5" s="24"/>
+      <c r="R5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="14"/>
-      <c r="T5" s="13" t="s">
+      <c r="S5" s="24"/>
+      <c r="T5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="U5" s="13" t="s">
+      <c r="U5" s="25" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
@@ -783,12 +840,12 @@
       <c r="I6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
       <c r="P6" s="12" t="s">
         <v>5</v>
       </c>
@@ -801,8 +858,8 @@
       <c r="S6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -1194,67 +1251,67 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="14">
         <v>11.8931</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="14">
         <v>12.122400000000001</v>
       </c>
-      <c r="D13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="30">
+      <c r="D13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="14">
         <v>12.7692</v>
       </c>
-      <c r="G13" s="30">
+      <c r="G13" s="14">
         <v>12.327500000000001</v>
       </c>
-      <c r="H13" s="30">
+      <c r="H13" s="14">
         <v>12.488799999999999</v>
       </c>
-      <c r="I13" s="30">
+      <c r="I13" s="14">
         <v>11.545500000000001</v>
       </c>
-      <c r="J13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="L13" s="30">
+      <c r="J13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="14">
         <v>14.611000000000001</v>
       </c>
-      <c r="M13" s="30">
+      <c r="M13" s="14">
         <v>15.1486</v>
       </c>
-      <c r="N13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="O13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="P13" s="30">
+      <c r="N13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" s="14">
         <v>15.7567</v>
       </c>
-      <c r="Q13" s="30">
+      <c r="Q13" s="14">
         <v>14.2964</v>
       </c>
-      <c r="R13" s="30">
+      <c r="R13" s="14">
         <v>14.9931</v>
       </c>
-      <c r="S13" s="30">
+      <c r="S13" s="14">
         <v>13.837400000000001</v>
       </c>
-      <c r="T13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="U13" s="29" t="s">
+      <c r="T13" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="U13" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1389,132 +1446,132 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="31">
+      <c r="B16" s="15">
         <v>15.230700000000001</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="14">
         <v>15.8794</v>
       </c>
-      <c r="D16" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="36">
+      <c r="D16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="20">
         <v>15.3744</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="15">
         <v>15.2136</v>
       </c>
-      <c r="H16" s="31">
+      <c r="H16" s="15">
         <v>15.010300000000001</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="15">
         <v>14.070600000000001</v>
       </c>
-      <c r="J16" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="K16" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="L16" s="30">
+      <c r="J16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="14">
         <v>18.652899999999999</v>
       </c>
-      <c r="M16" s="30">
+      <c r="M16" s="14">
         <v>19.4072</v>
       </c>
-      <c r="N16" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="O16" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="P16" s="31">
+      <c r="N16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="P16" s="15">
         <v>19.525500000000001</v>
       </c>
-      <c r="Q16" s="36">
+      <c r="Q16" s="20">
         <v>19.202500000000001</v>
       </c>
-      <c r="R16" s="30">
+      <c r="R16" s="14">
         <v>17.069099999999999</v>
       </c>
-      <c r="S16" s="31">
+      <c r="S16" s="15">
         <v>18.8599</v>
       </c>
-      <c r="T16" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="U16" s="29" t="s">
+      <c r="T16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="U16" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="34">
+      <c r="B17" s="18">
         <v>14.939500000000001</v>
       </c>
-      <c r="C17" s="37">
+      <c r="C17" s="21">
         <v>15.9551</v>
       </c>
-      <c r="D17" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="35">
+      <c r="D17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="19">
         <v>13.662800000000001</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="18">
         <v>13.752000000000001</v>
       </c>
-      <c r="H17" s="34">
+      <c r="H17" s="18">
         <v>13.3429</v>
       </c>
-      <c r="I17" s="34">
+      <c r="I17" s="18">
         <v>13.536799999999999</v>
       </c>
-      <c r="J17" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="L17" s="32">
+      <c r="J17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="16">
         <v>18.9712</v>
       </c>
-      <c r="M17" s="37">
+      <c r="M17" s="21">
         <v>19.6126</v>
       </c>
-      <c r="N17" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="O17" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="P17" s="34">
+      <c r="N17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="O17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="P17" s="18">
         <v>18.937200000000001</v>
       </c>
-      <c r="Q17" s="34">
+      <c r="Q17" s="18">
         <v>19.0989</v>
       </c>
-      <c r="R17" s="32">
+      <c r="R17" s="16">
         <v>17.856100000000001</v>
       </c>
-      <c r="S17" s="34">
+      <c r="S17" s="18">
         <v>17.753299999999999</v>
       </c>
-      <c r="T17" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="U17" s="33" t="s">
+      <c r="T17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="U17" s="17" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1698,7 +1755,7 @@
       <c r="Q20" s="7">
         <v>35.758699999999997</v>
       </c>
-      <c r="R20" s="38">
+      <c r="R20" s="22">
         <v>53.032899999999998</v>
       </c>
       <c r="S20" s="6">
@@ -1725,8 +1782,157 @@
         <v>28</v>
       </c>
     </row>
+    <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+    </row>
+    <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="C28">
+        <v>0.186</v>
+      </c>
+      <c r="D28">
+        <v>0.14599999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="C29">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="D29">
+        <v>0.223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>0.111</v>
+      </c>
+      <c r="C37">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="D37">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="E37" s="39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>0.111</v>
+      </c>
+      <c r="C38">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="D38">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="E38" s="39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41">
+        <v>1E-3</v>
+      </c>
+      <c r="C41">
+        <v>1E-3</v>
+      </c>
+      <c r="D41">
+        <v>1E-3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="26">
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:K4"/>
     <mergeCell ref="R5:S5"/>
     <mergeCell ref="T5:T6"/>
     <mergeCell ref="U5:U6"/>
@@ -1743,16 +1949,8 @@
     <mergeCell ref="P4:U4"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
results evaluation scripts added
</commit_message>
<xml_diff>
--- a/object_detection/TFLITE_PERF_TEST-COMPARISON.xlsx
+++ b/object_detection/TFLITE_PERF_TEST-COMPARISON.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ACCELR_internship\github\tflite-perf-tests\object_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAC715B-2D41-4980-B5C5-37E8BDC40AA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E20CBD-8368-4374-A2C8-16C53A58F397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="73">
   <si>
     <t>TFLITE-COMPARISON</t>
   </si>
@@ -133,21 +133,6 @@
     <t>IOU=0.75</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">AVERAGE PRECISION- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>BASELINES</t>
-    </r>
-  </si>
-  <si>
     <t>*add Dynamic, Static, etc</t>
   </si>
   <si>
@@ -157,9 +142,6 @@
     <t>mAP</t>
   </si>
   <si>
-    <t>* check model ZOO</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -203,6 +185,60 @@
   </si>
   <si>
     <t>0 (NA)</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>PROBLEM:</t>
+  </si>
+  <si>
+    <t>1. fps values were collected based on 0.6 threshold in PYTHON</t>
+  </si>
+  <si>
+    <t>2. fps values were collected using sample images of 5</t>
+  </si>
+  <si>
+    <t>mAP BASELINES</t>
+  </si>
+  <si>
+    <t>create FIGURE</t>
+  </si>
+  <si>
+    <t>mAP (IOU=0.50:0.95)</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. ssd_mobilenet_v2 (II- STATIC) </t>
+  </si>
+  <si>
+    <t>4. ssd_mobilenet_v1_1</t>
+  </si>
+  <si>
+    <t>32 bit-baselines (num_threads=1)</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>32bit C++</t>
+  </si>
+  <si>
+    <t>32bit Python</t>
+  </si>
+  <si>
+    <t>64bit C++</t>
+  </si>
+  <si>
+    <t>64bit Python</t>
+  </si>
+  <si>
+    <t>FPS</t>
+  </si>
+  <si>
+    <t>Experiment</t>
   </si>
 </sst>
 </file>
@@ -263,13 +299,6 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -283,6 +312,11 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -521,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -548,7 +582,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -558,25 +591,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -585,7 +616,7 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -602,15 +633,81 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -620,13 +717,28 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -634,14 +746,8 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -664,28 +770,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,6 +797,2351 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Frames</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Per Second (FPS)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AK$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1. ssd_mobilenet_v3_small</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AJ$67:$AJ$71</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32bit C++</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32bit Python</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64bit C++</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64bit Python</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AK$67:$AK$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.0786999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.9234000000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.9234000000000009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.9234000000000009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-77BB-4CBA-8E49-0CD46A3F3954}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AL$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2. ssd_mobilenet_v3_large</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AJ$67:$AJ$71</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32bit C++</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32bit Python</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64bit C++</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64bit Python</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AL$67:$AL$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.0070999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0617999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.7248999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-77BB-4CBA-8E49-0CD46A3F3954}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AM$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3. ssd_mobilenet_v2 (II- STATIC) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AJ$67:$AJ$71</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32bit C++</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32bit Python</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64bit C++</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64bit Python</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AM$67:$AM$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.9247000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.122400000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.327500000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.1486</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.2964</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-77BB-4CBA-8E49-0CD46A3F3954}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AN$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4. ssd_mobilenet_v1_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AJ$67:$AJ$71</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32bit C++</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32bit Python</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64bit C++</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64bit Python</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AN$67:$AN$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.3813000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.8794</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.2136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.4072</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.202500000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-77BB-4CBA-8E49-0CD46A3F3954}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1586219343"/>
+        <c:axId val="1290683231"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1586219343"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1290683231"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1290683231"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1586219343"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>COCO</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> mAP</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AQ$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1. ssd_mobilenet_v3_small</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AP$67:$AP$71</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32bit C++</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32bit Python</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64bit C++</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64bit Python</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AQ$67:$AQ$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.17799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17799999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-09F5-44AC-9327-AC46A6D54B23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AR$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2. ssd_mobilenet_v3_large</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AP$67:$AP$71</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32bit C++</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32bit Python</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64bit C++</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64bit Python</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AR$67:$AR$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-09F5-44AC-9327-AC46A6D54B23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AS$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3. ssd_mobilenet_v2 (II- STATIC) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AP$67:$AP$71</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32bit C++</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32bit Python</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64bit C++</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64bit Python</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AS$67:$AS$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14199999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-09F5-44AC-9327-AC46A6D54B23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AT$66</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4. ssd_mobilenet_v1_1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$AP$67:$AP$71</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>baseline</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32bit C++</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32bit Python</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64bit C++</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64bit Python</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AT$67:$AT$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-09F5-44AC-9327-AC46A6D54B23}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1577545967"/>
+        <c:axId val="1455771919"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1577545967"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1455771919"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1455771919"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1577545967"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>678492</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>68893</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FC4E981-7A22-4EF6-BB36-475A0AF40790}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>272233</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>77661</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA728671-C21E-4701-9C90-EFD18F91F8C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -905,10 +3345,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AL41"/>
+  <dimension ref="A1:AT71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="AE61" zoomScale="80" zoomScaleNormal="52" workbookViewId="0">
+      <selection activeCell="AU74" sqref="AU74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -936,353 +3376,357 @@
     <col min="28" max="28" width="14.44140625" customWidth="1"/>
     <col min="29" max="30" width="14.44140625" hidden="1" customWidth="1"/>
     <col min="32" max="35" width="14.44140625" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="28.6640625" customWidth="1"/>
+    <col min="37" max="37" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
-      <c r="AC1" s="65"/>
-      <c r="AD1" s="65"/>
-      <c r="AE1" s="65"/>
-      <c r="AF1" s="65"/>
-      <c r="AG1" s="65"/>
-      <c r="AH1" s="65"/>
-      <c r="AI1" s="65"/>
-    </row>
-    <row r="2" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91"/>
+      <c r="X1" s="91"/>
+      <c r="Y1" s="91"/>
+      <c r="Z1" s="91"/>
+      <c r="AA1" s="91"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="91"/>
+      <c r="AD1" s="91"/>
+      <c r="AE1" s="91"/>
+      <c r="AF1" s="91"/>
+      <c r="AG1" s="91"/>
+      <c r="AH1" s="91"/>
+      <c r="AI1" s="91"/>
+    </row>
+    <row r="2" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="64" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="78" t="s">
+      <c r="B2" s="86" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="44"/>
+      <c r="E2" s="84" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="85"/>
+      <c r="U2" s="85"/>
+      <c r="V2" s="85"/>
+      <c r="W2" s="85"/>
+      <c r="X2" s="85"/>
+      <c r="Y2" s="85"/>
+      <c r="Z2" s="85"/>
+      <c r="AA2" s="85"/>
+      <c r="AB2" s="85"/>
+      <c r="AC2" s="85"/>
+      <c r="AD2" s="85"/>
+      <c r="AE2" s="85"/>
+      <c r="AF2" s="44"/>
+      <c r="AG2" s="44"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="45"/>
+    </row>
+    <row r="3" spans="1:37" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="93"/>
+      <c r="S3" s="94"/>
+      <c r="T3" s="95" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" s="96"/>
+      <c r="V3" s="96"/>
+      <c r="W3" s="96"/>
+      <c r="X3" s="96"/>
+      <c r="Y3" s="96"/>
+      <c r="Z3" s="96"/>
+      <c r="AA3" s="96"/>
+      <c r="AB3" s="96"/>
+      <c r="AC3" s="96"/>
+      <c r="AD3" s="96"/>
+      <c r="AE3" s="96"/>
+      <c r="AF3" s="96"/>
+      <c r="AG3" s="96"/>
+      <c r="AH3" s="96"/>
+      <c r="AI3" s="97"/>
+    </row>
+    <row r="4" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="72"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="79" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="87" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="88"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="79" t="s">
+        <v>3</v>
+      </c>
+      <c r="U4" s="80"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="80"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="80"/>
+      <c r="AA4" s="87" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB4" s="88"/>
+      <c r="AC4" s="88"/>
+      <c r="AD4" s="88"/>
+      <c r="AE4" s="88"/>
+      <c r="AF4" s="88"/>
+      <c r="AG4" s="88"/>
+      <c r="AH4" s="88"/>
+      <c r="AI4" s="88"/>
+    </row>
+    <row r="5" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="72"/>
+      <c r="B5" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="72" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="73"/>
-      <c r="X2" s="73"/>
-      <c r="Y2" s="73"/>
-      <c r="Z2" s="73"/>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="73"/>
-      <c r="AC2" s="73"/>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="73"/>
-      <c r="AF2" s="76"/>
-      <c r="AG2" s="76"/>
-      <c r="AH2" s="76"/>
-      <c r="AI2" s="77"/>
-    </row>
-    <row r="3" spans="1:38" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="67"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="68"/>
-      <c r="T3" s="69" t="s">
-        <v>30</v>
-      </c>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="70"/>
-      <c r="X3" s="70"/>
-      <c r="Y3" s="70"/>
-      <c r="Z3" s="70"/>
-      <c r="AA3" s="70"/>
-      <c r="AB3" s="70"/>
-      <c r="AC3" s="70"/>
-      <c r="AD3" s="70"/>
-      <c r="AE3" s="70"/>
-      <c r="AF3" s="70"/>
-      <c r="AG3" s="70"/>
-      <c r="AH3" s="70"/>
-      <c r="AI3" s="71"/>
-    </row>
-    <row r="4" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="59" t="s">
-        <v>4</v>
-      </c>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="60"/>
-      <c r="S4" s="60"/>
-      <c r="T4" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="U4" s="58"/>
-      <c r="V4" s="58"/>
-      <c r="W4" s="58"/>
-      <c r="X4" s="58"/>
-      <c r="Y4" s="58"/>
-      <c r="Z4" s="58"/>
-      <c r="AA4" s="59" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB4" s="60"/>
-      <c r="AC4" s="60"/>
-      <c r="AD4" s="60"/>
-      <c r="AE4" s="60"/>
-      <c r="AF4" s="60"/>
-      <c r="AG4" s="60"/>
-      <c r="AH4" s="60"/>
-      <c r="AI4" s="60"/>
-    </row>
-    <row r="5" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="48"/>
-      <c r="B5" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="47" t="s">
+      <c r="F5" s="89" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="47" t="s">
+      <c r="J5" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="56" t="s">
+      <c r="K5" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="48"/>
-      <c r="M5" s="56" t="s">
+      <c r="L5" s="72"/>
+      <c r="M5" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="48"/>
-      <c r="O5" s="62" t="s">
-        <v>40</v>
-      </c>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="62"/>
-      <c r="R5" s="47" t="s">
+      <c r="N5" s="72"/>
+      <c r="O5" s="90" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5" s="90"/>
+      <c r="Q5" s="90"/>
+      <c r="R5" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="S5" s="47" t="s">
+      <c r="S5" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="T5" s="52" t="s">
+      <c r="T5" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="U5" s="54" t="s">
+      <c r="U5" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="V5" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="W5" s="61"/>
-      <c r="X5" s="61"/>
-      <c r="Y5" s="47" t="s">
+      <c r="V5" s="89" t="s">
+        <v>39</v>
+      </c>
+      <c r="W5" s="89"/>
+      <c r="X5" s="89"/>
+      <c r="Y5" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="Z5" s="47" t="s">
+      <c r="Z5" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="AA5" s="56" t="s">
+      <c r="AA5" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="AB5" s="48"/>
-      <c r="AC5" s="56" t="s">
+      <c r="AB5" s="72"/>
+      <c r="AC5" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="AD5" s="48"/>
-      <c r="AE5" s="62" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF5" s="62"/>
-      <c r="AG5" s="62"/>
-      <c r="AH5" s="47" t="s">
+      <c r="AD5" s="72"/>
+      <c r="AE5" s="90" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF5" s="90"/>
+      <c r="AG5" s="90"/>
+      <c r="AH5" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="AI5" s="47" t="s">
+      <c r="AI5" s="71" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
+    <row r="6" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="72"/>
       <c r="B6" s="63"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="20" t="s">
+      <c r="C6" s="62"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="22" t="s">
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="23" t="s">
+      <c r="L6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="22" t="s">
+      <c r="M6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="23" t="s">
+      <c r="N6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="O6" s="20" t="s">
+      <c r="O6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="P6" s="20" t="s">
+      <c r="P6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="Q6" s="20" t="s">
+      <c r="Q6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="R6" s="48"/>
-      <c r="S6" s="48"/>
-      <c r="T6" s="53"/>
-      <c r="U6" s="55"/>
-      <c r="V6" s="20" t="s">
+      <c r="R6" s="72"/>
+      <c r="S6" s="72"/>
+      <c r="T6" s="76"/>
+      <c r="U6" s="78"/>
+      <c r="V6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="W6" s="20" t="s">
+      <c r="W6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="X6" s="20" t="s">
+      <c r="X6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="Y6" s="48"/>
-      <c r="Z6" s="48"/>
-      <c r="AA6" s="22" t="s">
+      <c r="Y6" s="72"/>
+      <c r="Z6" s="72"/>
+      <c r="AA6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="AB6" s="23" t="s">
+      <c r="AB6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AC6" s="22" t="s">
+      <c r="AC6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="AD6" s="23" t="s">
+      <c r="AD6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AE6" s="20" t="s">
+      <c r="AE6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="AF6" s="20" t="s">
+      <c r="AF6" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="AG6" s="20" t="s">
+      <c r="AG6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AH6" s="48"/>
-      <c r="AI6" s="48"/>
-    </row>
-    <row r="7" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH6" s="72"/>
+      <c r="AI6" s="72"/>
+    </row>
+    <row r="7" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="42">
+      <c r="B7" s="39">
         <v>0.17799999999999999</v>
       </c>
-      <c r="C7" s="43"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="7">
         <v>8.5198999999999998</v>
       </c>
       <c r="E7" s="7">
         <v>8.9611999999999998</v>
       </c>
-      <c r="F7" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
+      <c r="F7" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
       <c r="I7" s="6" t="s">
         <v>12</v>
       </c>
@@ -1322,11 +3766,11 @@
       <c r="U7" s="7">
         <v>16.486599999999999</v>
       </c>
-      <c r="V7" s="41">
+      <c r="V7" s="38">
         <v>0</v>
       </c>
-      <c r="W7" s="31"/>
-      <c r="X7" s="31"/>
+      <c r="W7" s="28"/>
+      <c r="X7" s="28"/>
       <c r="Y7" s="6" t="s">
         <v>12</v>
       </c>
@@ -1361,25 +3805,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="42">
+      <c r="B8" s="39">
         <v>0.24</v>
       </c>
-      <c r="C8" s="43"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="7">
         <v>3.6566000000000001</v>
       </c>
       <c r="E8" s="7">
         <v>4.0309999999999997</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="28">
         <v>0</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
       <c r="I8" s="6" t="s">
         <v>12</v>
       </c>
@@ -1419,11 +3863,11 @@
       <c r="U8" s="7">
         <v>7.4348000000000001</v>
       </c>
-      <c r="V8" s="31">
+      <c r="V8" s="28">
         <v>0</v>
       </c>
-      <c r="W8" s="31"/>
-      <c r="X8" s="31"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="28"/>
       <c r="Y8" s="6" t="s">
         <v>12</v>
       </c>
@@ -1458,14 +3902,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="43"/>
+    <row r="9" spans="1:37" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="40"/>
       <c r="D9" s="6" t="s">
         <v>16</v>
       </c>
@@ -1529,11 +3973,11 @@
       <c r="AD9" s="7">
         <v>1.1094999999999999</v>
       </c>
-      <c r="AE9" s="31"/>
-      <c r="AF9" s="31">
+      <c r="AE9" s="28"/>
+      <c r="AF9" s="28">
         <v>0.17899999999999999</v>
       </c>
-      <c r="AG9" s="31">
+      <c r="AG9" s="28">
         <v>0.155</v>
       </c>
       <c r="AH9" s="6" t="s">
@@ -1543,14 +3987,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="43"/>
+    <row r="10" spans="1:37" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="40"/>
       <c r="D10" s="6" t="s">
         <v>16</v>
       </c>
@@ -1610,11 +4054,11 @@
       <c r="AD10" s="7">
         <v>1.294</v>
       </c>
-      <c r="AE10" s="31"/>
-      <c r="AF10" s="31">
+      <c r="AE10" s="28"/>
+      <c r="AF10" s="28">
         <v>0.17599999999999999</v>
       </c>
-      <c r="AG10" s="31">
+      <c r="AG10" s="28">
         <v>0.151</v>
       </c>
       <c r="AH10" s="6" t="s">
@@ -1624,14 +4068,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="43"/>
+    <row r="11" spans="1:37" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="40"/>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
@@ -1695,11 +4139,11 @@
       <c r="AD11" s="7">
         <v>4.1999000000000004</v>
       </c>
-      <c r="AE11" s="31"/>
-      <c r="AF11" s="31">
+      <c r="AE11" s="28"/>
+      <c r="AF11" s="28">
         <v>0.14099999999999999</v>
       </c>
-      <c r="AG11" s="31">
+      <c r="AG11" s="28">
         <v>0.11600000000000001</v>
       </c>
       <c r="AH11" s="6" t="s">
@@ -1709,23 +4153,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+    <row r="12" spans="1:37" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="43"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
       <c r="I12" s="10" t="s">
         <v>16</v>
       </c>
@@ -1780,11 +4224,11 @@
       <c r="AD12" s="7">
         <v>4.9962999999999997</v>
       </c>
-      <c r="AE12" s="31"/>
-      <c r="AF12" s="31">
+      <c r="AE12" s="28"/>
+      <c r="AF12" s="28">
         <v>0.13200000000000001</v>
       </c>
-      <c r="AG12" s="31">
+      <c r="AG12" s="28">
         <v>0.108</v>
       </c>
       <c r="AH12" s="6" t="s">
@@ -1795,29 +4239,28 @@
       </c>
       <c r="AJ12" s="3"/>
       <c r="AK12" s="3"/>
-      <c r="AL12" s="3"/>
-    </row>
-    <row r="13" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="44">
+    </row>
+    <row r="13" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="41">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C13" s="43"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="12">
         <v>11.8931</v>
       </c>
       <c r="E13" s="12">
         <v>12.122400000000001</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="23">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="23">
         <v>0.20399999999999999</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="23">
         <v>0.13900000000000001</v>
       </c>
       <c r="I13" s="11" t="s">
@@ -1902,14 +4345,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="43"/>
+    <row r="14" spans="1:37" ht="13.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="40"/>
       <c r="D14" s="6" t="s">
         <v>16</v>
       </c>
@@ -1973,11 +4416,11 @@
       <c r="AD14" s="7">
         <v>0.27600000000000002</v>
       </c>
-      <c r="AE14" s="31"/>
-      <c r="AF14" s="31">
+      <c r="AE14" s="28"/>
+      <c r="AF14" s="28">
         <v>0.14099999999999999</v>
       </c>
-      <c r="AG14" s="31">
+      <c r="AG14" s="28">
         <v>0.13200000000000001</v>
       </c>
       <c r="AH14" s="6" t="s">
@@ -1987,14 +4430,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:38" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="43"/>
+    <row r="15" spans="1:37" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="40"/>
       <c r="D15" s="6" t="s">
         <v>16</v>
       </c>
@@ -2058,11 +4501,11 @@
       <c r="AD15" s="7">
         <v>0.1111</v>
       </c>
-      <c r="AE15" s="31"/>
-      <c r="AF15" s="31">
+      <c r="AE15" s="28"/>
+      <c r="AF15" s="28">
         <v>0.14899999999999999</v>
       </c>
-      <c r="AG15" s="31">
+      <c r="AG15" s="28">
         <v>0.13900000000000001</v>
       </c>
       <c r="AH15" s="6" t="s">
@@ -2072,27 +4515,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="42">
+      <c r="B16" s="39">
         <v>0.14799999999999999</v>
       </c>
-      <c r="C16" s="43"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="13">
         <v>15.230700000000001</v>
       </c>
       <c r="E16" s="12">
         <v>15.8794</v>
       </c>
-      <c r="F16" s="24">
+      <c r="F16" s="23">
         <v>0.14799999999999999</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="23">
         <v>0.23300000000000001</v>
       </c>
-      <c r="H16" s="24">
+      <c r="H16" s="23">
         <v>0.154</v>
       </c>
       <c r="I16" s="11" t="s">
@@ -2101,7 +4544,7 @@
       <c r="J16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="15">
+      <c r="K16" s="14">
         <v>15.3744</v>
       </c>
       <c r="L16" s="13">
@@ -2152,7 +4595,7 @@
       <c r="AA16" s="13">
         <v>19.525500000000001</v>
       </c>
-      <c r="AB16" s="15">
+      <c r="AB16" s="14">
         <v>19.202500000000001</v>
       </c>
       <c r="AC16" s="12">
@@ -2178,101 +4621,101 @@
       </c>
     </row>
     <row r="17" spans="1:35" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="45" t="s">
-        <v>50</v>
+      <c r="B17" s="42" t="s">
+        <v>48</v>
       </c>
       <c r="C17">
         <v>0.111</v>
       </c>
-      <c r="D17" s="35">
+      <c r="D17" s="32">
         <v>14.939500000000001</v>
       </c>
-      <c r="E17" s="36">
+      <c r="E17" s="33">
         <v>15.9551</v>
       </c>
-      <c r="F17" s="37">
+      <c r="F17" s="34">
         <v>0.14799999999999999</v>
       </c>
-      <c r="G17" s="37">
+      <c r="G17" s="34">
         <v>0.23300000000000001</v>
       </c>
-      <c r="H17" s="37">
+      <c r="H17" s="34">
         <v>0.154</v>
       </c>
-      <c r="I17" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="38">
+      <c r="I17" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="35">
         <v>13.662800000000001</v>
       </c>
-      <c r="L17" s="35">
+      <c r="L17" s="32">
         <v>13.752000000000001</v>
       </c>
-      <c r="M17" s="35">
+      <c r="M17" s="32">
         <v>13.3429</v>
       </c>
-      <c r="N17" s="35">
+      <c r="N17" s="32">
         <v>13.536799999999999</v>
       </c>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="S17" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="T17" s="39">
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="R17" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="S17" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="T17" s="36">
         <v>18.9712</v>
       </c>
-      <c r="U17" s="36">
+      <c r="U17" s="33">
         <v>19.6126</v>
       </c>
-      <c r="V17" s="36">
+      <c r="V17" s="33">
         <v>0.14699999999999999</v>
       </c>
-      <c r="W17" s="36">
+      <c r="W17" s="33">
         <v>0.23300000000000001</v>
       </c>
-      <c r="X17" s="36">
+      <c r="X17" s="33">
         <v>0.154</v>
       </c>
-      <c r="Y17" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z17" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA17" s="35">
+      <c r="Y17" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z17" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA17" s="32">
         <v>18.937200000000001</v>
       </c>
-      <c r="AB17" s="35">
+      <c r="AB17" s="32">
         <v>19.0989</v>
       </c>
-      <c r="AC17" s="39">
+      <c r="AC17" s="36">
         <v>17.856100000000001</v>
       </c>
-      <c r="AD17" s="35">
+      <c r="AD17" s="32">
         <v>17.753299999999999</v>
       </c>
-      <c r="AE17" s="40"/>
-      <c r="AF17" s="40">
+      <c r="AE17" s="37"/>
+      <c r="AF17" s="37">
         <v>0.16500000000000001</v>
       </c>
-      <c r="AG17" s="40">
+      <c r="AG17" s="37">
         <v>0.11799999999999999</v>
       </c>
-      <c r="AH17" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI17" s="34" t="s">
+      <c r="AH17" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI17" s="31" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2280,10 +4723,10 @@
       <c r="A18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="18"/>
+      <c r="B18" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="17"/>
       <c r="D18" s="7">
         <v>12.8</v>
       </c>
@@ -2347,11 +4790,11 @@
       <c r="AD18" s="7">
         <v>14.2798</v>
       </c>
-      <c r="AE18" s="31"/>
-      <c r="AF18" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG18" s="31" t="s">
+      <c r="AE18" s="28"/>
+      <c r="AF18" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG18" s="28" t="s">
         <v>16</v>
       </c>
       <c r="AH18" s="6" t="s">
@@ -2365,8 +4808,8 @@
       <c r="A19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="45" t="s">
-        <v>50</v>
+      <c r="B19" s="42" t="s">
+        <v>48</v>
       </c>
       <c r="D19" s="7">
         <v>14.7342</v>
@@ -2429,9 +4872,9 @@
         <v>16</v>
       </c>
       <c r="AD19" s="7"/>
-      <c r="AE19" s="31"/>
-      <c r="AF19" s="31"/>
-      <c r="AG19" s="31"/>
+      <c r="AE19" s="28"/>
+      <c r="AF19" s="28"/>
+      <c r="AG19" s="28"/>
       <c r="AH19" s="6" t="s">
         <v>16</v>
       </c>
@@ -2440,14 +4883,14 @@
       </c>
     </row>
     <row r="20" spans="1:35" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>42</v>
+      <c r="B20" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="D20" s="7">
         <v>31.8306</v>
@@ -2506,17 +4949,17 @@
       <c r="AB20" s="7">
         <v>35.758699999999997</v>
       </c>
-      <c r="AC20" s="16">
+      <c r="AC20" s="15">
         <v>53.032899999999998</v>
       </c>
       <c r="AD20" s="6">
         <v>40.878900000000002</v>
       </c>
-      <c r="AE20" s="32"/>
-      <c r="AF20" s="33">
+      <c r="AE20" s="29"/>
+      <c r="AF20" s="30">
         <v>1E-3</v>
       </c>
-      <c r="AG20" s="33">
+      <c r="AG20" s="30">
         <v>1E-3</v>
       </c>
       <c r="AH20" s="6" t="s">
@@ -2527,7 +4970,7 @@
       </c>
     </row>
     <row r="21" spans="1:35" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B21" s="46"/>
+      <c r="B21" s="43"/>
       <c r="U21" s="1"/>
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
@@ -2549,52 +4992,48 @@
       <c r="C24" s="5"/>
     </row>
     <row r="26" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="49" t="s">
+      <c r="B26" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="69"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="19" t="s">
+      <c r="K26" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="K26" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="L26" s="21" t="s">
-        <v>41</v>
-      </c>
+      <c r="L26" s="47"/>
     </row>
     <row r="27" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18" t="s">
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17" t="s">
         <v>36</v>
       </c>
       <c r="L27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
+      <c r="B28" s="39">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="C28" s="25"/>
       <c r="D28">
         <v>0.13900000000000001</v>
-      </c>
-      <c r="E28">
-        <v>0.186</v>
       </c>
       <c r="I28">
         <v>0.14599999999999999</v>
@@ -2604,94 +5043,101 @@
       <c r="A29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
+      <c r="B29" s="39">
+        <v>0.24</v>
+      </c>
+      <c r="C29" s="25"/>
       <c r="D29">
         <v>0.20100000000000001</v>
       </c>
-      <c r="E29">
-        <v>0.27400000000000002</v>
-      </c>
       <c r="I29">
         <v>0.223</v>
       </c>
-    </row>
-    <row r="30" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L29" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:35" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-    </row>
-    <row r="31" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+    </row>
+    <row r="31" spans="1:35" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-    </row>
-    <row r="32" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="1:35" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-    </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+    </row>
+    <row r="33" spans="1:41" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+    </row>
+    <row r="34" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="27"/>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="B34" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="46"/>
+      <c r="L34" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:41" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
+    </row>
+    <row r="36" spans="1:41" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="B36" s="46"/>
+      <c r="C36" s="46"/>
+    </row>
+    <row r="37" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
+      <c r="B37" s="39">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="C37" s="46"/>
       <c r="D37">
         <v>0.111</v>
       </c>
-      <c r="E37">
-        <v>0.16500000000000001</v>
-      </c>
       <c r="I37">
         <v>0.11799999999999999</v>
       </c>
-      <c r="J37" s="17" t="s">
+      <c r="J37" s="16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="L37" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:41" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
+      <c r="B38" s="46"/>
+      <c r="C38" s="46"/>
       <c r="D38">
         <v>0.111</v>
       </c>
@@ -2701,30 +5147,30 @@
       <c r="I38">
         <v>0.11799999999999999</v>
       </c>
-      <c r="J38" s="17" t="s">
+      <c r="J38" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+    <row r="39" spans="1:41" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="B39" s="46"/>
+      <c r="C39" s="46"/>
+    </row>
+    <row r="40" spans="1:41" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-    </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+      <c r="B40" s="46"/>
+      <c r="C40" s="46"/>
+    </row>
+    <row r="41" spans="1:41" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
       <c r="D41">
         <v>1E-3</v>
       </c>
@@ -2735,12 +5181,505 @@
         <v>1E-3</v>
       </c>
     </row>
+    <row r="42" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="43"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
+    </row>
+    <row r="45" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ45" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK45" s="68"/>
+      <c r="AL45" s="68"/>
+      <c r="AM45" s="68"/>
+      <c r="AN45" s="68"/>
+      <c r="AO45" s="68"/>
+    </row>
+    <row r="46" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ46" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK46" s="67" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL46" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM46" s="65"/>
+      <c r="AN46" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO46" s="66"/>
+    </row>
+    <row r="47" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ47" s="64"/>
+      <c r="AK47" s="67"/>
+      <c r="AL47" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM47" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN47" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO47" s="52" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ48" s="64"/>
+      <c r="AK48" s="67"/>
+      <c r="AL48" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM48" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN48" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO48" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ49" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK49" s="39">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="AL49" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM49" s="7">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="AN49" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO49" s="7">
+        <v>0.17799999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ50" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK50" s="39">
+        <v>0.24</v>
+      </c>
+      <c r="AL50" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM50" s="7">
+        <v>0.24</v>
+      </c>
+      <c r="AN50" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO50" s="7">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="51" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ51" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK51" s="41">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AL51" s="23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AM51" s="12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AN51" s="12">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AO51" s="12">
+        <v>0.14199999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ52" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK52" s="39">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="AL52" s="23">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="AM52" s="13">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="AN52" s="12">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="AO52" s="13">
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ53" s="42"/>
+      <c r="AK53" s="46"/>
+      <c r="AL53" s="53"/>
+      <c r="AM53" s="54"/>
+      <c r="AN53" s="54"/>
+      <c r="AO53" s="54"/>
+    </row>
+    <row r="54" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ54" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK54" s="68"/>
+      <c r="AL54" s="68"/>
+      <c r="AM54" s="68"/>
+      <c r="AN54" s="68"/>
+      <c r="AO54" s="68"/>
+    </row>
+    <row r="55" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ55" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK55" s="67" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL55" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM55" s="65"/>
+      <c r="AN55" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO55" s="66"/>
+    </row>
+    <row r="56" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ56" s="64"/>
+      <c r="AK56" s="67"/>
+      <c r="AL56" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM56" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN56" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO56" s="52" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="36:41" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ57" s="64"/>
+      <c r="AK57" s="67"/>
+      <c r="AL57" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM57" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="AN57" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="AO57" s="50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ58" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK58" s="39"/>
+      <c r="AL58" s="7">
+        <v>8.9611999999999998</v>
+      </c>
+      <c r="AM58" s="7">
+        <v>8.9234000000000009</v>
+      </c>
+      <c r="AN58" s="7">
+        <v>16.486599999999999</v>
+      </c>
+      <c r="AO58" s="7">
+        <v>19.9146</v>
+      </c>
+    </row>
+    <row r="59" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ59" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK59" s="39"/>
+      <c r="AL59" s="7">
+        <v>4.0309999999999997</v>
+      </c>
+      <c r="AM59" s="7">
+        <v>4.0617999999999999</v>
+      </c>
+      <c r="AN59" s="7">
+        <v>7.4348000000000001</v>
+      </c>
+      <c r="AO59" s="7">
+        <v>8.7248999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ60" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK60" s="41"/>
+      <c r="AL60" s="12">
+        <v>12.122400000000001</v>
+      </c>
+      <c r="AM60" s="12">
+        <v>12.327500000000001</v>
+      </c>
+      <c r="AN60" s="12">
+        <v>15.1486</v>
+      </c>
+      <c r="AO60" s="12">
+        <v>14.2964</v>
+      </c>
+    </row>
+    <row r="61" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ61" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK61" s="39"/>
+      <c r="AL61" s="12">
+        <v>15.8794</v>
+      </c>
+      <c r="AM61" s="13">
+        <v>15.2136</v>
+      </c>
+      <c r="AN61" s="12">
+        <v>19.4072</v>
+      </c>
+      <c r="AO61" s="14">
+        <v>19.202500000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="36:46" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ65" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK65" s="60"/>
+      <c r="AL65" s="60"/>
+      <c r="AM65" s="60"/>
+      <c r="AN65" s="60"/>
+      <c r="AP65" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ65" s="60"/>
+      <c r="AR65" s="60"/>
+      <c r="AS65" s="60"/>
+      <c r="AT65" s="60"/>
+    </row>
+    <row r="66" spans="36:46" ht="44.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ66" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK66" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL66" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="AM66" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN66" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP66" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ66" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR66" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="AS66" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="AT66" s="57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="36:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ67" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK67" s="59">
+        <v>8.0786999999999995</v>
+      </c>
+      <c r="AL67" s="59">
+        <v>3.0070999999999999</v>
+      </c>
+      <c r="AM67" s="98">
+        <v>3.9247000000000001</v>
+      </c>
+      <c r="AN67" s="59">
+        <v>5.3813000000000004</v>
+      </c>
+      <c r="AO67" s="99"/>
+      <c r="AP67" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ67" s="59">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="AR67" s="59">
+        <v>0.24</v>
+      </c>
+      <c r="AS67" s="58">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AT67" s="59">
+        <v>0.14799999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="36:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ68" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK68" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL68" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM68" s="59">
+        <v>12.122400000000001</v>
+      </c>
+      <c r="AN68" s="59">
+        <v>15.8794</v>
+      </c>
+      <c r="AO68" s="99"/>
+      <c r="AP68" s="101" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ68" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR68" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS68" s="58">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AT68" s="58">
+        <v>0.14799999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="36:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ69" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK69" s="59">
+        <v>8.9234000000000009</v>
+      </c>
+      <c r="AL69" s="59">
+        <v>4.0617999999999999</v>
+      </c>
+      <c r="AM69" s="59">
+        <v>12.327500000000001</v>
+      </c>
+      <c r="AN69" s="59">
+        <v>15.2136</v>
+      </c>
+      <c r="AO69" s="99"/>
+      <c r="AP69" s="101" t="s">
+        <v>68</v>
+      </c>
+      <c r="AQ69" s="59">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="AR69" s="59">
+        <v>0.24</v>
+      </c>
+      <c r="AS69" s="59">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AT69" s="59">
+        <v>0.14799999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="36:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ70" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK70" s="59">
+        <v>8.9234000000000009</v>
+      </c>
+      <c r="AL70" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM70" s="59">
+        <v>15.1486</v>
+      </c>
+      <c r="AN70" s="59">
+        <v>19.4072</v>
+      </c>
+      <c r="AO70" s="99"/>
+      <c r="AP70" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ70" s="100" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR70" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS70" s="59">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AT70" s="59">
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="36:46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AJ71" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK71" s="59">
+        <v>8.9234000000000009</v>
+      </c>
+      <c r="AL71" s="59">
+        <v>8.7248999999999999</v>
+      </c>
+      <c r="AM71" s="59">
+        <v>14.2964</v>
+      </c>
+      <c r="AN71" s="59">
+        <v>19.202500000000001</v>
+      </c>
+      <c r="AO71" s="99"/>
+      <c r="AP71" s="101" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ71" s="59">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="AR71" s="59">
+        <v>0.24</v>
+      </c>
+      <c r="AS71" s="59">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AT71" s="59">
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="E2:AE2"/>
-    <mergeCell ref="B2:B4"/>
+  <mergeCells count="46">
     <mergeCell ref="A1:AI1"/>
     <mergeCell ref="T5:T6"/>
     <mergeCell ref="U5:U6"/>
@@ -2757,22 +5696,39 @@
     <mergeCell ref="AE5:AG5"/>
     <mergeCell ref="AH5:AH6"/>
     <mergeCell ref="AI5:AI6"/>
-    <mergeCell ref="D26:I26"/>
-    <mergeCell ref="S5:S6"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="AC5:AD5"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:L5"/>
     <mergeCell ref="D4:J4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="E2:AE2"/>
+    <mergeCell ref="B2:B4"/>
     <mergeCell ref="K4:S4"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="AJ65:AN65"/>
+    <mergeCell ref="AP65:AT65"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B5:B6"/>
+    <mergeCell ref="AJ55:AJ57"/>
+    <mergeCell ref="AL55:AM55"/>
+    <mergeCell ref="AN55:AO55"/>
+    <mergeCell ref="AJ46:AJ48"/>
+    <mergeCell ref="AL46:AM46"/>
+    <mergeCell ref="AN46:AO46"/>
+    <mergeCell ref="AK55:AK57"/>
+    <mergeCell ref="AK46:AK48"/>
+    <mergeCell ref="AJ45:AO45"/>
+    <mergeCell ref="AJ54:AO54"/>
+    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="S5:S6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
results updated, minor changes
</commit_message>
<xml_diff>
--- a/object_detection/TFLITE_PERF_TEST-COMPARISON.xlsx
+++ b/object_detection/TFLITE_PERF_TEST-COMPARISON.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ACCELR_internship\github\tflite-perf-tests\object_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3251403-BD15-40C9-BCFD-546917B95B7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25CA348-85C1-4731-8A9C-AF4BF5D7FFAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9924" yWindow="84" windowWidth="12480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -717,39 +717,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -761,55 +791,25 @@
     <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3377,8 +3377,8 @@
   </sheetPr>
   <dimension ref="A1:AZ79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V59" zoomScale="73" zoomScaleNormal="52" workbookViewId="0">
-      <selection activeCell="AN69" sqref="AN69"/>
+    <sheetView tabSelected="1" topLeftCell="AJ58" zoomScale="59" zoomScaleNormal="52" workbookViewId="0">
+      <selection activeCell="AS76" sqref="AS76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3411,262 +3411,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
-      <c r="AE1" s="70"/>
-      <c r="AF1" s="70"/>
-      <c r="AG1" s="70"/>
-      <c r="AH1" s="70"/>
-      <c r="AI1" s="70"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="100"/>
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
+      <c r="W1" s="100"/>
+      <c r="X1" s="100"/>
+      <c r="Y1" s="100"/>
+      <c r="Z1" s="100"/>
+      <c r="AA1" s="100"/>
+      <c r="AB1" s="100"/>
+      <c r="AC1" s="100"/>
+      <c r="AD1" s="100"/>
+      <c r="AE1" s="100"/>
+      <c r="AF1" s="100"/>
+      <c r="AG1" s="100"/>
+      <c r="AH1" s="100"/>
+      <c r="AI1" s="100"/>
     </row>
     <row r="2" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="91" t="s">
+      <c r="C2" s="90" t="s">
         <v>53</v>
       </c>
       <c r="D2" s="44"/>
-      <c r="E2" s="94" t="s">
+      <c r="E2" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
-      <c r="Q2" s="95"/>
-      <c r="R2" s="95"/>
-      <c r="S2" s="95"/>
-      <c r="T2" s="95"/>
-      <c r="U2" s="95"/>
-      <c r="V2" s="95"/>
-      <c r="W2" s="95"/>
-      <c r="X2" s="95"/>
-      <c r="Y2" s="95"/>
-      <c r="Z2" s="95"/>
-      <c r="AA2" s="95"/>
-      <c r="AB2" s="95"/>
-      <c r="AC2" s="95"/>
-      <c r="AD2" s="95"/>
-      <c r="AE2" s="95"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="94"/>
+      <c r="R2" s="94"/>
+      <c r="S2" s="94"/>
+      <c r="T2" s="94"/>
+      <c r="U2" s="94"/>
+      <c r="V2" s="94"/>
+      <c r="W2" s="94"/>
+      <c r="X2" s="94"/>
+      <c r="Y2" s="94"/>
+      <c r="Z2" s="94"/>
+      <c r="AA2" s="94"/>
+      <c r="AB2" s="94"/>
+      <c r="AC2" s="94"/>
+      <c r="AD2" s="94"/>
+      <c r="AE2" s="94"/>
       <c r="AF2" s="44"/>
       <c r="AG2" s="44"/>
       <c r="AH2" s="44"/>
       <c r="AI2" s="45"/>
     </row>
     <row r="3" spans="1:37" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="90"/>
-      <c r="B3" s="96"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="80" t="s">
+      <c r="A3" s="83"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
-      <c r="Q3" s="81"/>
-      <c r="R3" s="81"/>
-      <c r="S3" s="82"/>
-      <c r="T3" s="83" t="s">
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
+      <c r="O3" s="102"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="102"/>
+      <c r="R3" s="102"/>
+      <c r="S3" s="103"/>
+      <c r="T3" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="U3" s="84"/>
-      <c r="V3" s="84"/>
-      <c r="W3" s="84"/>
-      <c r="X3" s="84"/>
-      <c r="Y3" s="84"/>
-      <c r="Z3" s="84"/>
-      <c r="AA3" s="84"/>
-      <c r="AB3" s="84"/>
-      <c r="AC3" s="84"/>
-      <c r="AD3" s="84"/>
-      <c r="AE3" s="84"/>
-      <c r="AF3" s="84"/>
-      <c r="AG3" s="84"/>
-      <c r="AH3" s="84"/>
-      <c r="AI3" s="85"/>
+      <c r="U3" s="105"/>
+      <c r="V3" s="105"/>
+      <c r="W3" s="105"/>
+      <c r="X3" s="105"/>
+      <c r="Y3" s="105"/>
+      <c r="Z3" s="105"/>
+      <c r="AA3" s="105"/>
+      <c r="AB3" s="105"/>
+      <c r="AC3" s="105"/>
+      <c r="AD3" s="105"/>
+      <c r="AE3" s="105"/>
+      <c r="AF3" s="105"/>
+      <c r="AG3" s="105"/>
+      <c r="AH3" s="105"/>
+      <c r="AI3" s="106"/>
     </row>
     <row r="4" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="78" t="s">
+      <c r="A4" s="81"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="86" t="s">
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="87"/>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="87"/>
-      <c r="T4" s="78" t="s">
+      <c r="L4" s="97"/>
+      <c r="M4" s="97"/>
+      <c r="N4" s="97"/>
+      <c r="O4" s="97"/>
+      <c r="P4" s="97"/>
+      <c r="Q4" s="97"/>
+      <c r="R4" s="97"/>
+      <c r="S4" s="97"/>
+      <c r="T4" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="79"/>
-      <c r="Z4" s="79"/>
-      <c r="AA4" s="86" t="s">
+      <c r="U4" s="89"/>
+      <c r="V4" s="89"/>
+      <c r="W4" s="89"/>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="87"/>
-      <c r="AE4" s="87"/>
-      <c r="AF4" s="87"/>
-      <c r="AG4" s="87"/>
-      <c r="AH4" s="87"/>
-      <c r="AI4" s="87"/>
+      <c r="AB4" s="97"/>
+      <c r="AC4" s="97"/>
+      <c r="AD4" s="97"/>
+      <c r="AE4" s="97"/>
+      <c r="AF4" s="97"/>
+      <c r="AG4" s="97"/>
+      <c r="AH4" s="97"/>
+      <c r="AI4" s="97"/>
     </row>
     <row r="5" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="76"/>
-      <c r="B5" s="99" t="s">
+      <c r="A5" s="81"/>
+      <c r="B5" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="97" t="s">
+      <c r="C5" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="71" t="s">
+      <c r="D5" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="73" t="s">
+      <c r="E5" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="88" t="s">
+      <c r="F5" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="75" t="s">
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="75" t="s">
+      <c r="J5" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="77" t="s">
+      <c r="K5" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="76"/>
-      <c r="M5" s="77" t="s">
+      <c r="L5" s="81"/>
+      <c r="M5" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="76"/>
-      <c r="O5" s="89" t="s">
+      <c r="N5" s="81"/>
+      <c r="O5" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="P5" s="89"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="75" t="s">
+      <c r="P5" s="99"/>
+      <c r="Q5" s="99"/>
+      <c r="R5" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="S5" s="75" t="s">
+      <c r="S5" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="T5" s="71" t="s">
+      <c r="T5" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="U5" s="73" t="s">
+      <c r="U5" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="V5" s="88" t="s">
+      <c r="V5" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="W5" s="88"/>
-      <c r="X5" s="88"/>
-      <c r="Y5" s="75" t="s">
+      <c r="W5" s="98"/>
+      <c r="X5" s="98"/>
+      <c r="Y5" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="Z5" s="75" t="s">
+      <c r="Z5" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="AA5" s="77" t="s">
+      <c r="AA5" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="AB5" s="76"/>
-      <c r="AC5" s="77" t="s">
+      <c r="AB5" s="81"/>
+      <c r="AC5" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="AD5" s="76"/>
-      <c r="AE5" s="89" t="s">
+      <c r="AD5" s="81"/>
+      <c r="AE5" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="AF5" s="89"/>
-      <c r="AG5" s="89"/>
-      <c r="AH5" s="75" t="s">
+      <c r="AF5" s="99"/>
+      <c r="AG5" s="99"/>
+      <c r="AH5" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="AI5" s="75" t="s">
+      <c r="AI5" s="80" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="76"/>
-      <c r="B6" s="99"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="74"/>
+      <c r="A6" s="81"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="87"/>
       <c r="F6" s="19" t="s">
         <v>34</v>
       </c>
@@ -3676,8 +3676,8 @@
       <c r="H6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
       <c r="K6" s="21" t="s">
         <v>5</v>
       </c>
@@ -3699,10 +3699,10 @@
       <c r="Q6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="R6" s="76"/>
-      <c r="S6" s="76"/>
-      <c r="T6" s="72"/>
-      <c r="U6" s="74"/>
+      <c r="R6" s="81"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="85"/>
+      <c r="U6" s="87"/>
       <c r="V6" s="19" t="s">
         <v>34</v>
       </c>
@@ -3712,8 +3712,8 @@
       <c r="X6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="Y6" s="76"/>
-      <c r="Z6" s="76"/>
+      <c r="Y6" s="81"/>
+      <c r="Z6" s="81"/>
       <c r="AA6" s="21" t="s">
         <v>5</v>
       </c>
@@ -3735,8 +3735,8 @@
       <c r="AG6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="AH6" s="76"/>
-      <c r="AI6" s="76"/>
+      <c r="AH6" s="81"/>
+      <c r="AI6" s="81"/>
     </row>
     <row r="7" spans="1:37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -5025,12 +5025,12 @@
       <c r="B26" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="105"/>
-      <c r="E26" s="106"/>
-      <c r="F26" s="106"/>
-      <c r="G26" s="106"/>
-      <c r="H26" s="106"/>
-      <c r="I26" s="106"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="79"/>
+      <c r="I26" s="79"/>
       <c r="J26" s="18" t="s">
         <v>37</v>
       </c>
@@ -5220,34 +5220,34 @@
       <c r="A45" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="AJ45" s="104" t="s">
+      <c r="AJ45" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="AK45" s="104"/>
-      <c r="AL45" s="104"/>
-      <c r="AM45" s="104"/>
-      <c r="AN45" s="104"/>
-      <c r="AO45" s="104"/>
+      <c r="AK45" s="77"/>
+      <c r="AL45" s="77"/>
+      <c r="AM45" s="77"/>
+      <c r="AN45" s="77"/>
+      <c r="AO45" s="77"/>
     </row>
     <row r="46" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AJ46" s="100" t="s">
+      <c r="AJ46" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="AK46" s="103" t="s">
+      <c r="AK46" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="AL46" s="101" t="s">
+      <c r="AL46" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="AM46" s="101"/>
-      <c r="AN46" s="102" t="s">
+      <c r="AM46" s="74"/>
+      <c r="AN46" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="AO46" s="102"/>
+      <c r="AO46" s="75"/>
     </row>
     <row r="47" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AJ47" s="100"/>
-      <c r="AK47" s="103"/>
+      <c r="AJ47" s="73"/>
+      <c r="AK47" s="76"/>
       <c r="AL47" s="51" t="s">
         <v>3</v>
       </c>
@@ -5262,8 +5262,8 @@
       </c>
     </row>
     <row r="48" spans="1:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AJ48" s="100"/>
-      <c r="AK48" s="103"/>
+      <c r="AJ48" s="73"/>
+      <c r="AK48" s="76"/>
       <c r="AL48" s="19" t="s">
         <v>61</v>
       </c>
@@ -5366,34 +5366,34 @@
       <c r="AO53" s="54"/>
     </row>
     <row r="54" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AJ54" s="104" t="s">
+      <c r="AJ54" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="AK54" s="104"/>
-      <c r="AL54" s="104"/>
-      <c r="AM54" s="104"/>
-      <c r="AN54" s="104"/>
-      <c r="AO54" s="104"/>
+      <c r="AK54" s="77"/>
+      <c r="AL54" s="77"/>
+      <c r="AM54" s="77"/>
+      <c r="AN54" s="77"/>
+      <c r="AO54" s="77"/>
     </row>
     <row r="55" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AJ55" s="100" t="s">
+      <c r="AJ55" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="AK55" s="103" t="s">
+      <c r="AK55" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="AL55" s="101" t="s">
+      <c r="AL55" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="AM55" s="101"/>
-      <c r="AN55" s="102" t="s">
+      <c r="AM55" s="74"/>
+      <c r="AN55" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="AO55" s="102"/>
+      <c r="AO55" s="75"/>
     </row>
     <row r="56" spans="36:41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AJ56" s="100"/>
-      <c r="AK56" s="103"/>
+      <c r="AJ56" s="73"/>
+      <c r="AK56" s="76"/>
       <c r="AL56" s="51" t="s">
         <v>3</v>
       </c>
@@ -5408,8 +5408,8 @@
       </c>
     </row>
     <row r="57" spans="36:41" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AJ57" s="100"/>
-      <c r="AK57" s="103"/>
+      <c r="AJ57" s="73"/>
+      <c r="AK57" s="76"/>
       <c r="AL57" s="19" t="s">
         <v>6</v>
       </c>
@@ -5918,6 +5918,38 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="AV73:AZ73"/>
+    <mergeCell ref="AV65:AZ65"/>
+    <mergeCell ref="A1:AI1"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="U5:U6"/>
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="T4:Z4"/>
+    <mergeCell ref="D3:S3"/>
+    <mergeCell ref="T3:AI3"/>
+    <mergeCell ref="AA4:AI4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="AE5:AG5"/>
+    <mergeCell ref="AH5:AH6"/>
+    <mergeCell ref="AI5:AI6"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="E2:AE2"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K4:S4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="O5:Q5"/>
     <mergeCell ref="AJ65:AN65"/>
     <mergeCell ref="AP65:AT65"/>
     <mergeCell ref="C5:C6"/>
@@ -5934,38 +5966,6 @@
     <mergeCell ref="AJ54:AO54"/>
     <mergeCell ref="D26:I26"/>
     <mergeCell ref="S5:S6"/>
-    <mergeCell ref="AH5:AH6"/>
-    <mergeCell ref="AI5:AI6"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="E2:AE2"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K4:S4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="AV73:AZ73"/>
-    <mergeCell ref="AV65:AZ65"/>
-    <mergeCell ref="A1:AI1"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="Y5:Y6"/>
-    <mergeCell ref="Z5:Z6"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="T4:Z4"/>
-    <mergeCell ref="D3:S3"/>
-    <mergeCell ref="T3:AI3"/>
-    <mergeCell ref="AA4:AI4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="V5:X5"/>
-    <mergeCell ref="AE5:AG5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>